<commit_message>
feat: enhance document number normalization and ubigeo handling in client import
</commit_message>
<xml_diff>
--- a/app/web/public/plantillas/Plantilla_ImportacionClientes_basico.xlsx
+++ b/app/web/public/plantillas/Plantilla_ImportacionClientes_basico.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://contasisitc-my.sharepoint.com/personal/a_huaman_contasiscorp_com/Documents/Clientes BC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FacturaFacil\app\web\public\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="8_{76C8F1A7-B56B-4E20-90E8-157BA47884D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0995C90E-C4F8-47E7-A116-2D22E9707969}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1140347F-5D5F-4C13-AAA7-F47FFE3F0D09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -308,7 +308,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -348,6 +348,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -364,10 +366,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -659,14 +657,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.21875" customWidth="1"/>
-    <col min="2" max="3" width="28.33203125" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" customWidth="1"/>
+    <col min="3" max="3" width="28.33203125" style="18" customWidth="1"/>
     <col min="4" max="4" width="25.88671875" customWidth="1"/>
     <col min="5" max="8" width="23.44140625" customWidth="1"/>
     <col min="9" max="9" width="17.109375" customWidth="1"/>
@@ -684,7 +683,7 @@
       <c r="B1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="17" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -728,7 +727,7 @@
       <c r="B2">
         <v>6</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="18">
         <v>23656985698</v>
       </c>
       <c r="D2" t="s">
@@ -754,7 +753,7 @@
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="18">
         <v>56856985</v>
       </c>
       <c r="E3" t="s">

</xml_diff>